<commit_message>
Updates to the Budget and scheduler
</commit_message>
<xml_diff>
--- a/public/import/inventorybudgets.xlsx
+++ b/public/import/inventorybudgets.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bakasa\code\php\laravel\blowplast\public\import\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D41C49-700A-483B-B87B-72250B2DF9A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F8839EA2-3742-4CBB-8C74-7A904D1816EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Pieces" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -473,11 +467,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
@@ -657,51 +651,51 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -718,7 +712,7 @@
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{F1A995F4-2592-4A72-ACEA-6E365A150AB1}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -791,7 +785,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -843,7 +837,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1037,18 +1031,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D52FA9DB-7B45-41C9-9C30-1EA57A4CC22E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="J1" sqref="J1:U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>